<commit_message>
Updating IMS assay metadata
</commit_message>
<xml_diff>
--- a/desi/latest/desi.xlsx
+++ b/desi/latest/desi.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="355">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -285,6 +285,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000246</t>
   </si>
   <si>
+    <t>MIBI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
+  </si>
+  <si>
     <t>DESI</t>
   </si>
   <si>
@@ -345,12 +351,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000222</t>
   </si>
   <si>
-    <t>Multiplex Ion Beam Imaging</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -588,12 +588,6 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
-    <t>Bruker Daltonics</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023608</t>
-  </si>
-  <si>
     <t>Standard BioTools (Fluidigm)</t>
   </si>
   <si>
@@ -606,6 +600,12 @@
     <t>https://identifiers.org/RRID:SCR_023651</t>
   </si>
   <si>
+    <t>Bruker</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_017365</t>
+  </si>
+  <si>
     <t>Keyence</t>
   </si>
   <si>
@@ -930,6 +930,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000281</t>
   </si>
   <si>
+    <t>HESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000289</t>
+  </si>
+  <si>
     <t>LA</t>
   </si>
   <si>
@@ -954,6 +960,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000280</t>
   </si>
   <si>
+    <t>ESI</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C19363</t>
+  </si>
+  <si>
     <t>MALDI-2</t>
   </si>
   <si>
@@ -1089,6 +1101,12 @@
     <t>preparation_instrument_vendor</t>
   </si>
   <si>
+    <t>In-House</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
     <t>HTX Technologies</t>
   </si>
   <si>
@@ -1101,12 +1119,6 @@
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
-  </si>
-  <si>
     <t>SunChrom</t>
   </si>
   <si>
@@ -1266,7 +1278,7 @@
     <t>desorption_solvent_flow_rate_unit</t>
   </si>
   <si>
-    <t>μL/min</t>
+    <t>uL/min</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000271</t>
@@ -1299,7 +1311,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-18T12:04:42-07:00</t>
+    <t>2023-10-20T20:01:10-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1490,57 +1502,57 @@
         <v>220</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2">
       <c r="AE2" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1587,7 @@
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'ms_ionization_technique'!$A$1:$A$8</formula1>
+      <formula1>'ms_ionization_technique'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'ms_scan_mode'!$A$1:$A$3</formula1>
@@ -1641,26 +1653,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1678,26 +1690,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1715,50 +1727,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1776,42 +1788,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1829,58 +1841,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>282</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -1906,26 +1918,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
@@ -1946,66 +1958,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B8" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B10" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B11" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2023,58 +2035,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B7" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2092,50 +2104,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B6" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -2153,18 +2165,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -2188,30 +2200,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C1" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3162,7 +3174,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3202,23 +3214,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>232</v>
@@ -3230,6 +3242,22 @@
       </c>
       <c r="B8" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update IMS metadata templates to use updated descriptions
</commit_message>
<xml_diff>
--- a/desi/latest/desi.xlsx
+++ b/desi/latest/desi.xlsx
@@ -38,106 +38,112 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
@@ -244,8 +250,8 @@
     </comment>
     <comment ref="AE1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -254,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="510">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -280,34 +286,172 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -316,36 +460,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -376,16 +490,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -394,24 +502,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -442,18 +538,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -466,12 +550,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -484,34 +562,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -649,6 +709,18 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -763,12 +835,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -802,6 +886,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -910,6 +1000,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -988,6 +1084,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1024,6 +1126,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1114,6 +1222,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1138,6 +1249,18 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1150,6 +1273,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1174,6 +1303,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1291,6 +1426,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000279</t>
   </si>
   <si>
+    <t>nESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000456</t>
+  </si>
+  <si>
     <t>ms_scan_mode</t>
   </si>
   <si>
@@ -1642,7 +1783,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:16:13-07:00</t>
+    <t>2025-10-20T10:54:03-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1800,85 +1941,85 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>345</v>
+        <v>390</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>352</v>
+        <v>397</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>359</v>
+        <v>404</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>360</v>
+        <v>405</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>361</v>
+        <v>406</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>362</v>
+        <v>407</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>363</v>
+        <v>408</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>376</v>
+        <v>421</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>385</v>
+        <v>430</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>392</v>
+        <v>437</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>419</v>
+        <v>464</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>436</v>
+        <v>481</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>449</v>
+        <v>494</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>455</v>
+        <v>500</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>456</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2">
@@ -1886,13 +2027,13 @@
         <v>12</v>
       </c>
       <c r="AE2" t="s" s="32">
-        <v>457</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="24">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1901,10 +2042,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1921,7 +2062,7 @@
       <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'ms_ionization_technique'!$A$1:$A$10</formula1>
+      <formula1>'ms_ionization_technique'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'ms_scan_mode'!$A$1:$A$3</formula1>
@@ -1987,26 +2128,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>346</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>347</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>349</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>350</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>351</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -2024,26 +2165,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>398</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>400</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -2061,50 +2202,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>365</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>366</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>367</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>368</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>369</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>371</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>372</v>
+        <v>417</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>373</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>374</v>
+        <v>419</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>375</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -2122,42 +2263,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>377</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>378</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>383</v>
+        <v>428</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>384</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -2175,74 +2316,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>386</v>
+        <v>431</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>387</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>388</v>
+        <v>433</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>389</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>170</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>172</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>390</v>
+        <v>435</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>391</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -2260,146 +2401,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>393</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>394</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>395</v>
+        <v>440</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>396</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>233</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>299</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>397</v>
+        <v>442</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>398</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>399</v>
+        <v>444</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>400</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>401</v>
+        <v>446</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>402</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>403</v>
+        <v>448</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>404</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>405</v>
+        <v>450</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>406</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>407</v>
+        <v>452</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>408</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>409</v>
+        <v>454</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>410</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>411</v>
+        <v>456</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>412</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>413</v>
+        <v>458</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>414</v>
+        <v>459</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>415</v>
+        <v>460</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>416</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>417</v>
+        <v>462</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>418</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -2417,66 +2558,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>420</v>
+        <v>465</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>421</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>422</v>
+        <v>467</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>423</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>424</v>
+        <v>469</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>425</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>426</v>
+        <v>471</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>427</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>428</v>
+        <v>473</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>429</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>430</v>
+        <v>475</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>431</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>432</v>
+        <v>477</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>433</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>434</v>
+        <v>479</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>435</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -2494,50 +2635,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>437</v>
+        <v>482</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>438</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>439</v>
+        <v>484</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>440</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>441</v>
+        <v>486</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>442</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>443</v>
+        <v>488</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>444</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>446</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>447</v>
+        <v>492</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>448</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -2555,18 +2696,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>451</v>
+        <v>496</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>452</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>453</v>
+        <v>498</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>454</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -2590,16 +2731,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>458</v>
+        <v>503</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>459</v>
+        <v>504</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>461</v>
+        <v>506</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>463</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
@@ -2607,13 +2748,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>460</v>
+        <v>505</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>462</v>
+        <v>507</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>464</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -2623,7 +2764,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2955,6 +3096,78 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2972,130 +3185,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3113,12 +3326,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3341,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3136,210 +3349,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3349,7 +3594,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3357,546 +3602,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3914,42 +4231,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3967,26 +4284,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3996,7 +4313,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4004,50 +4321,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>370</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>328</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>329</v>
+        <v>372</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>330</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>331</v>
+        <v>374</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>332</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>333</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>334</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>335</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>336</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>337</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7">
@@ -4055,31 +4372,39 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>338</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>339</v>
+        <v>382</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>340</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>341</v>
+        <v>384</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>342</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>344</v>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>388</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-update IMS metadata templates to use updated field descriptions
</commit_message>
<xml_diff>
--- a/desi/latest/desi.xlsx
+++ b/desi/latest/desi.xlsx
@@ -148,25 +148,27 @@
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) The ionization approach (i.e., sample probing method) for performing
-imaging mass spectrometry.</t>
+        <t>(Required) The ionization technique used in imaging mass spectrometry, which
+refers to the method employed to probe the sample. Example: MALDI</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) MS (mass spectrometry) scan mode refers to the number of steps in the
-separation of fragments.</t>
+        <t>(Required) The mode of mass spectrometry (MS) scanning, which refers to the
+number of steps involved in the separation of fragments during the analysis.
+Example: MS1</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The polarity of the mass analysis (positive or negative ion modes).</t>
+        <t>(Required) The polarity mode used in mass analysis, indicating whether positive
+or negative ion modes are employed. Example: Positive ion mode</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) The low value of the scanned mass-to-charge range, for MS1.
-(unitless)</t>
+        <t>(Required) The low value of the scanned mass-to-charge range for MS1. This value
+is unitless. Example: 100</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
@@ -177,68 +179,76 @@
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>(Required) The mass resolving power m/∆m, where ∆m is defined as the full width
-at half-maximum (FWHM) for a given peak with a specified mass-to-charge (m/z).
-(unitless)</t>
+        <t>(Required) The mass resolving power, denoted as m/∆m, where ∆m is defined as the
+full width at half-maximum (FWHM) for a given peak with a specified
+mass-to-charge ratio (m/z). This measurement is unitless. Example: 60000</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>(Required) The peak (m/z) used to calculate the resolving power.</t>
+        <t>(Required) The peak mass-to-charge ratio (m/z) used to calculate the resolving
+power. Example: 400.2</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>Specifies which technology was used for ion mobility spectrometry. Technologies
-for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS),
-Trapped Ion Mobility Spectrometry (TIMS), High Field Asymmetric waveform ion
-Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS),
-Structures for Lossless Ion Manipulations (SLIM), and cyclic Ion Mobility
-Spectrometry (cIMS).</t>
+        <t>The specific technology employed for ion mobility spectrometry. Available
+technologies include Traveling Wave Ion Mobility Spectrometry (TWIMS), Trapped
+Ion Mobility Spectrometry (TIMS), High Field Asymmetric Waveform Ion Mobility
+Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS), Structures
+for Lossless Ion Manipulations (SLIM), and cyclic Ion Mobility Spectrometry
+(cIMS). Example: TIMS</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>Common methods of depositing matrix for assisting in desorption and ionization
-in imaging mass spectrometry include robotic spotting, electrospray deposition,
-and sublimation.</t>
+        <t>The method used for matrix deposition to aid in desorption and ionization in
+imaging mass spectrometry. Common techniques include robotic spotting,
+electrospray deposition, and sublimation. Example: Robotic spraying</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>The manufacturer of the instrument used to prepare (staining/processing) the
-sample for the assay. If an automatic slide staining method was indicated this
-field should list the manufacturer of the instrument.</t>
+        <t>The company that manufactures the instrument used to prepare the sample (e.g.,
+for staining or other processing steps) prior to the assay. If the instrument
+was custom-built or developed internally, enter "In-House". If no sample
+preparation occurred, enter "Not applicable". Example: 10X Genomics</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>Manufacturers of a staining system instrument may offer various versions
-(models) of that instrument with different features. Differences in features or
-sensitivities may be relevant to processing or interpretation of the data.</t>
+        <t>The specific model of the instrument used for sample preparation, such as
+staining. Manufacturers may offer multiple models with varying features or
+sensitivities, which can influence how the sample is processed and how the
+resulting data is interpreted. If no sample preparation occurred, enter "Not
+applicable". Example: Chromium X</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>The matrix is a compound of crystallized molecules that acts like a buffer
-between the sample and the ionizing probe. It also helps ionize the sample,
-carrying it along the flight tube so it can be detected.</t>
+        <t>The preparation matrix, which is a compound of crystallized molecules that
+functions as a buffer between the sample and the ionizing probe. This matrix
+also aids in ionizing the sample, facilitating its movement along the flight
+tube for detection. Example: DMACA (4-(dimethylamino)cinnamic acid)</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>(Required) Solvent composition for conducting nanospray desorption electrospray
-ionization (nanoDESI) or desorption electrospray ionization (DESI).</t>
+        <t>(Required) The composition of the solvent used for conducting nanospray
+desorption electrospray ionization (nanoDESI) or desorption electrospray
+ionization (DESI). Example: Ethanol:Dimethylformamide (EtOH:DMF)</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>(Required) The rate of flow of the solvent into a spray.</t>
+        <t>(Required) The rate at which the solvent flows into a spray. Example: 1.5</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>(Required) Units of the rate of solvent flow.</t>
+        <t>(Required) The unit of measurement for the desorption solvent flow rate value.
+If the flow rate is not applicable or not measured, this field may be left
+blank. Example: uL/min</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
@@ -1783,7 +1793,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-20T10:54:03-07:00</t>
+    <t>2025-10-20T15:17:40-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
fix: Add new categorical values
</commit_message>
<xml_diff>
--- a/desi/latest/desi.xlsx
+++ b/desi/latest/desi.xlsx
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="530">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -572,6 +572,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
   </si>
   <si>
+    <t>Raman Imaging</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000475</t>
+  </si>
+  <si>
     <t>RNAseq (with probes)</t>
   </si>
   <si>
@@ -584,6 +590,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
+    <t>STARmap</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000476</t>
+  </si>
+  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -857,6 +869,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -986,6 +1004,12 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -1028,6 +1052,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1154,6 +1184,12 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1295,6 +1331,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -1811,7 +1853,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-20T09:43:53-08:00</t>
+    <t>2025-12-15T11:35:09-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1969,85 +2011,85 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>501</v>
+        <v>515</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>506</v>
+        <v>520</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>507</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2">
@@ -2055,13 +2097,13 @@
         <v>12</v>
       </c>
       <c r="AE2" t="s" s="32">
-        <v>508</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="24">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$51</formula1>
+      <formula1>'dataset_type'!$A$1:$A$53</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$17</formula1>
@@ -2070,10 +2112,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$81</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2156,26 +2198,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>396</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>398</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>400</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2193,26 +2235,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>403</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>405</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>407</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -2230,50 +2272,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>414</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>416</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>418</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>420</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>422</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>424</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -2291,42 +2333,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>427</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>429</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>431</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>433</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -2344,90 +2386,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>436</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>438</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>440</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -2445,154 +2487,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>443</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>445</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>447</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>344</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>449</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>451</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>453</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>455</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>457</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>459</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>461</v>
+        <v>475</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>463</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>465</v>
+        <v>479</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>466</v>
+        <v>480</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>467</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>469</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -2610,66 +2652,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>472</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>474</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>476</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>478</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>480</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>482</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>484</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>486</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2687,50 +2729,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>489</v>
+        <v>503</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>491</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>493</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>495</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>497</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>498</v>
+        <v>512</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>499</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -2748,18 +2790,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>502</v>
+        <v>516</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>503</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>505</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -2783,16 +2825,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>510</v>
+        <v>524</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>512</v>
+        <v>526</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>514</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2">
@@ -2800,13 +2842,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>513</v>
+        <v>527</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>515</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -2816,7 +2858,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3228,6 +3270,22 @@
       </c>
       <c r="B51" t="s" s="0">
         <v>105</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3245,138 +3303,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3394,12 +3452,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3409,7 +3467,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3417,242 +3475,250 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3662,7 +3728,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3670,618 +3736,650 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>70</v>
+        <v>330</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>328</v>
+        <v>335</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>329</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>175</v>
+        <v>337</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>335</v>
+        <v>179</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>336</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>356</v>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -4299,42 +4397,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>368</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4352,26 +4450,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>364</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4389,42 +4487,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>375</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>377</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>379</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>381</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>383</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6">
@@ -4432,7 +4530,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>384</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
@@ -4440,39 +4538,39 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>385</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>387</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>391</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>393</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>